<commit_message>
updated OSC mapping and added PDF version
</commit_message>
<xml_diff>
--- a/patches/gum/OSC-mapping.xlsx
+++ b/patches/gum/OSC-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roboos/eegsynth/patches/gum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F14938A-C030-7D4D-9645-4EF1E4DA12F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E438A125-43C8-A642-B905-260CE48F4F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="3580" windowWidth="28040" windowHeight="17440" xr2:uid="{588B919B-CA89-A84E-9506-EC1D751CEB63}"/>
+    <workbookView xWindow="1480" yWindow="1020" windowWidth="28040" windowHeight="17440" xr2:uid="{588B919B-CA89-A84E-9506-EC1D751CEB63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,18 +238,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -257,20 +251,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,208 +656,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2C93FA-0FE6-9F43-A089-FA626875F79E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="100.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="103.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58.83203125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>40</v>
       </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="14"/>
+    </row>
+    <row r="4" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="16" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="14"/>
+    </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="14"/>
+    </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B23" s="14"/>
+    </row>
+    <row r="24" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="16" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="14"/>
+    </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B28" s="14"/>
+    </row>
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="17" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="76" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>